<commit_message>
run 15 74 p won remove normalization
</commit_message>
<xml_diff>
--- a/logs.xlsx
+++ b/logs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\delta-2\Desktop\PingPongPlayingRobotSimulation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D7A24D4-E73D-4D08-A8C3-4954BA938461}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26BF04ED-FBC9-4446-B78E-46D006C29A97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13290" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="41">
   <si>
     <t>run_id</t>
   </si>
@@ -147,10 +147,14 @@
     <t>08% won</t>
   </si>
   <si>
+    <t>remove observation normalization</t>
+  </si>
+  <si>
+    <t>34%
+t=41%</t>
+  </si>
+  <si>
     <t>?</t>
-  </si>
-  <si>
-    <t>remove observation normalization</t>
   </si>
 </sst>
 </file>
@@ -192,9 +196,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -479,8 +486,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L335"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+    <sheetView tabSelected="1" topLeftCell="C13" workbookViewId="0">
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1063,97 +1070,130 @@
       <c r="J15" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="K15" s="1" t="s">
-        <v>38</v>
+      <c r="K15" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="L15" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
+      <c r="B16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="1">
+        <v>128</v>
+      </c>
+      <c r="D16" s="1">
+        <v>50000</v>
+      </c>
+      <c r="E16" s="1">
+        <v>3</v>
+      </c>
+      <c r="F16" s="1">
+        <v>8</v>
+      </c>
+      <c r="G16" s="1">
+        <v>5000000</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K16" s="2">
+        <v>0.74</v>
+      </c>
       <c r="L16" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="L17" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -2676,5 +2716,6 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
courtB collision set to on trigger run 17
</commit_message>
<xml_diff>
--- a/logs.xlsx
+++ b/logs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\delta-2\Desktop\PingPongPlayingRobotSimulation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26BF04ED-FBC9-4446-B78E-46D006C29A97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07D8C015-8F0C-4104-9141-1EA5E1DE0714}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13290" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="44">
   <si>
     <t>run_id</t>
   </si>
@@ -154,7 +154,20 @@
 t=41%</t>
   </si>
   <si>
-    <t>?</t>
+    <t>first hit = 1
+other hit = 0
+else = 0</t>
+  </si>
+  <si>
+    <t>detect the first collision between racket and ball</t>
+  </si>
+  <si>
+    <t>hit = 1
+hit opponent court = 5
+else = 0</t>
+  </si>
+  <si>
+    <t>collision of opponent court set to ontrigger</t>
   </si>
 </sst>
 </file>
@@ -486,8 +499,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L335"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C13" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1115,17 +1128,77 @@
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>16</v>
       </c>
+      <c r="B17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="1">
+        <v>128</v>
+      </c>
+      <c r="D17" s="1">
+        <v>50000</v>
+      </c>
+      <c r="E17" s="1">
+        <v>3</v>
+      </c>
+      <c r="F17" s="1">
+        <v>8</v>
+      </c>
+      <c r="G17" s="1">
+        <v>5000000</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K17" s="2">
+        <v>0.09</v>
+      </c>
       <c r="L17" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>17</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="1">
+        <v>128</v>
+      </c>
+      <c r="D18" s="1">
+        <v>50000</v>
+      </c>
+      <c r="E18" s="1">
+        <v>3</v>
+      </c>
+      <c r="F18" s="1">
+        <v>8</v>
+      </c>
+      <c r="G18" s="1">
+        <v>5000000</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
racket only actions rotation and position
</commit_message>
<xml_diff>
--- a/logs.xlsx
+++ b/logs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\delta-2\Desktop\PingPongPlayingRobotSimulation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07D8C015-8F0C-4104-9141-1EA5E1DE0714}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43B39CF6-572A-41A7-9CD4-A245A7CB8F70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13290" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="63">
   <si>
     <t>run_id</t>
   </si>
@@ -168,6 +168,76 @@
   </si>
   <si>
     <t>collision of opponent court set to ontrigger</t>
+  </si>
+  <si>
+    <t>17%
+opp_won=5%</t>
+  </si>
+  <si>
+    <t>hit = 10
+hit opponent court = 10
+else = 0</t>
+  </si>
+  <si>
+    <t>equalizing the reward function for hit and court</t>
+  </si>
+  <si>
+    <t>27%
+opp_won=5%</t>
+  </si>
+  <si>
+    <t>add racket rotation to observation and actions</t>
+  </si>
+  <si>
+    <t>change position</t>
+  </si>
+  <si>
+    <t>rotate angles
+&amp; change position</t>
+  </si>
+  <si>
+    <t>36%
+opp_won=5%</t>
+  </si>
+  <si>
+    <t>change stack vector to 15</t>
+  </si>
+  <si>
+    <t>46%
+opp_won=5%</t>
+  </si>
+  <si>
+    <t>Solved first hit problem</t>
+  </si>
+  <si>
+    <t>56%
+opp_won=10%</t>
+  </si>
+  <si>
+    <t>45%
+opp_won=7%</t>
+  </si>
+  <si>
+    <t>adding rotation to observation</t>
+  </si>
+  <si>
+    <t>?%
+opp_won=?%</t>
+  </si>
+  <si>
+    <t>hit = 1
+hit opponent court = 10
+else =01</t>
+  </si>
+  <si>
+    <t>dynamic reward for hit and court</t>
+  </si>
+  <si>
+    <t>5%
+opp_won=5%</t>
+  </si>
+  <si>
+    <t>add speed to observation &amp; change decision period to 4</t>
   </si>
 </sst>
 </file>
@@ -499,8 +569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L335"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -520,7 +590,7 @@
     <col min="13" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1113,7 +1183,7 @@
         <v>5000000</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>12</v>
+        <v>49</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>25</v>
@@ -1151,7 +1221,7 @@
         <v>5000000</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>12</v>
+        <v>49</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>25</v>
@@ -1189,7 +1259,7 @@
         <v>5000000</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>12</v>
+        <v>49</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>25</v>
@@ -1197,53 +1267,320 @@
       <c r="J18" s="1" t="s">
         <v>42</v>
       </c>
+      <c r="K18" s="2" t="s">
+        <v>44</v>
+      </c>
       <c r="L18" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" s="1">
+        <v>128</v>
+      </c>
+      <c r="D19" s="1">
+        <v>50000</v>
+      </c>
+      <c r="E19" s="1">
+        <v>3</v>
+      </c>
+      <c r="F19" s="1">
+        <v>8</v>
+      </c>
+      <c r="G19" s="1">
+        <v>5000000</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B20" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" s="1">
+        <v>128</v>
+      </c>
+      <c r="D20" s="1">
+        <v>50000</v>
+      </c>
+      <c r="E20" s="1">
+        <v>3</v>
+      </c>
+      <c r="F20" s="1">
+        <v>8</v>
+      </c>
+      <c r="G20" s="1">
+        <v>5000000</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B21" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" s="1">
+        <v>128</v>
+      </c>
+      <c r="D21" s="1">
+        <v>50000</v>
+      </c>
+      <c r="E21" s="1">
+        <v>3</v>
+      </c>
+      <c r="F21" s="1">
+        <v>8</v>
+      </c>
+      <c r="G21" s="1">
+        <v>5000000</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K21" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B22" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="1">
+        <v>128</v>
+      </c>
+      <c r="D22" s="1">
+        <v>50000</v>
+      </c>
+      <c r="E22" s="1">
+        <v>3</v>
+      </c>
+      <c r="F22" s="1">
+        <v>128</v>
+      </c>
+      <c r="G22" s="1">
+        <v>5000000</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K22" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B23" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" s="1">
+        <v>128</v>
+      </c>
+      <c r="D23" s="1">
+        <v>50000</v>
+      </c>
+      <c r="E23" s="1">
+        <v>3</v>
+      </c>
+      <c r="F23" s="1">
+        <v>128</v>
+      </c>
+      <c r="G23" s="1">
+        <v>5000000</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B24" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C24" s="1">
+        <v>128</v>
+      </c>
+      <c r="D24" s="1">
+        <v>50000</v>
+      </c>
+      <c r="E24" s="1">
+        <v>3</v>
+      </c>
+      <c r="F24" s="1">
+        <v>128</v>
+      </c>
+      <c r="G24" s="1">
+        <v>5000000</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K24" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B25" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25" s="1">
+        <v>128</v>
+      </c>
+      <c r="D25" s="1">
+        <v>50000</v>
+      </c>
+      <c r="E25" s="1">
+        <v>3</v>
+      </c>
+      <c r="F25" s="1">
+        <v>128</v>
+      </c>
+      <c r="G25" s="1">
+        <v>5000000</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>25</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26" s="1">
+        <v>128</v>
+      </c>
+      <c r="D26" s="1">
+        <v>50000</v>
+      </c>
+      <c r="E26" s="1">
+        <v>3</v>
+      </c>
+      <c r="F26" s="1">
+        <v>128</v>
+      </c>
+      <c r="G26" s="1">
+        <v>5000000</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L26" s="1" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>26</v>
+      </c>
+      <c r="L27" s="1" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>